<commit_message>
fixing sample excel files + report values
</commit_message>
<xml_diff>
--- a/frontend/src/resources/jbook-ai-inv-sample.xlsx
+++ b/frontend/src/resources/jbook-ai-inv-sample.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/usmanqadri/Documents/gamechanger-web-source/frontend/src/resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ryanchan/Projects/gamechanger-web/frontend/src/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8820FB03-F407-0249-B891-412FBAD16FE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38824D27-D324-4944-BB3F-73F1987FA457}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="900" yWindow="760" windowWidth="32000" windowHeight="19060" xr2:uid="{91155129-0587-1B4A-A8D0-D1CB89AEEB30}"/>
+    <workbookView xWindow="41680" yWindow="8360" windowWidth="32000" windowHeight="19060" xr2:uid="{91155129-0587-1B4A-A8D0-D1CB89AEEB30}"/>
   </bookViews>
   <sheets>
     <sheet name="Primary Review Worksheet" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t>Primary Reviewer</t>
   </si>
@@ -89,27 +89,6 @@
     <t>Project # (RDT&amp;E Only)</t>
   </si>
   <si>
-    <t>Total Funding</t>
-  </si>
-  <si>
-    <t>BY1 Funding</t>
-  </si>
-  <si>
-    <t>BY2 Funding</t>
-  </si>
-  <si>
-    <t>BY3 Funding</t>
-  </si>
-  <si>
-    <t>BY4 Funding</t>
-  </si>
-  <si>
-    <t>BY5 Funding</t>
-  </si>
-  <si>
-    <t>Has Keywords</t>
-  </si>
-  <si>
     <t>AI Analysis</t>
   </si>
   <si>
@@ -117,6 +96,45 @@
   </si>
   <si>
     <t>Department</t>
+  </si>
+  <si>
+    <t>Agency / Office</t>
+  </si>
+  <si>
+    <t>RAI Secondary Reviewer</t>
+  </si>
+  <si>
+    <t>RAI Tag Agree</t>
+  </si>
+  <si>
+    <t>RAI Tag</t>
+  </si>
+  <si>
+    <t>RAI Transition Partner Agree</t>
+  </si>
+  <si>
+    <t>RAI Transition Partner</t>
+  </si>
+  <si>
+    <t>RAI Mission Partners</t>
+  </si>
+  <si>
+    <t>POC Title</t>
+  </si>
+  <si>
+    <t>POC Name</t>
+  </si>
+  <si>
+    <t>POC Email</t>
+  </si>
+  <si>
+    <t>POC Org</t>
+  </si>
+  <si>
+    <t>POC Phone Number</t>
+  </si>
+  <si>
+    <t>RAI Review Notes</t>
   </si>
 </sst>
 </file>
@@ -480,20 +498,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52895EAF-BBA6-5048-B092-D84C951CDB4B}">
-  <dimension ref="A1:AA1"/>
+  <dimension ref="A1:AG1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="X18" sqref="X18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:27" s="1" customFormat="1" ht="96" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:33" s="1" customFormat="1" ht="96" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -505,7 +523,7 @@
         <v>3</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>4</v>
@@ -526,7 +544,7 @@
         <v>9</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="N1" s="1" t="s">
         <v>10</v>
@@ -550,25 +568,43 @@
         <v>16</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="X1" s="1" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="Y1" s="1" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="Z1" s="1" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="AA1" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AF1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AG1" s="1" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>